<commit_message>
tidying up Dookie sims and data
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/DookieEVA2024.xlsx
+++ b/Tests/Validation/Wheat/data/DookieEVA2024.xlsx
@@ -46,6 +46,9 @@
     <t>Wheat.AboveGround.Wt</t>
   </si>
   <si>
+    <t>Wheat.Ear.Wt</t>
+  </si>
+  <si>
     <t>Wheat.Grain.Wt</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
   </si>
   <si>
     <t>Wheat.Grain.Number</t>
-  </si>
-  <si>
-    <t>Wheat.Ear.Wt</t>
   </si>
   <si>
     <t>SimulationName</t>
@@ -1767,7 +1767,7 @@
         <v>45559</v>
       </c>
       <c r="D116">
-        <v>14</v>
+        <v>13.875</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2284,7 +2284,7 @@
         <v>45559</v>
       </c>
       <c r="D163">
-        <v>11</v>
+        <v>10.66666666666667</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2383,7 +2383,7 @@
         <v>45559</v>
       </c>
       <c r="D172">
-        <v>11.875</v>
+        <v>11.66666666666667</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2482,7 +2482,7 @@
         <v>45559</v>
       </c>
       <c r="D181">
-        <v>11.75</v>
+        <v>11.58333333333333</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -2606,7 +2606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:12">
+    <row r="193" spans="1:13">
       <c r="A193" s="1" t="s">
         <v>19</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:12">
+    <row r="194" spans="1:13">
       <c r="A194" s="1" t="s">
         <v>20</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:12">
+    <row r="195" spans="1:13">
       <c r="A195" s="1" t="s">
         <v>21</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:12">
+    <row r="196" spans="1:13">
       <c r="A196" s="1" t="s">
         <v>22</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:12">
+    <row r="197" spans="1:13">
       <c r="A197" s="1" t="s">
         <v>23</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:12">
+    <row r="198" spans="1:13">
       <c r="A198" s="1" t="s">
         <v>16</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:12">
+    <row r="199" spans="1:13">
       <c r="A199" s="1" t="s">
         <v>17</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:12">
+    <row r="200" spans="1:13">
       <c r="A200" s="1" t="s">
         <v>18</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:12">
+    <row r="201" spans="1:13">
       <c r="A201" s="1" t="s">
         <v>19</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:12">
+    <row r="202" spans="1:13">
       <c r="A202" s="1" t="s">
         <v>20</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:12">
+    <row r="203" spans="1:13">
       <c r="A203" s="1" t="s">
         <v>21</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:12">
+    <row r="204" spans="1:13">
       <c r="A204" s="1" t="s">
         <v>22</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:12">
+    <row r="205" spans="1:13">
       <c r="A205" s="1" t="s">
         <v>23</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:12">
+    <row r="206" spans="1:13">
       <c r="A206" s="1" t="s">
         <v>16</v>
       </c>
@@ -2780,8 +2780,11 @@
       <c r="L206">
         <v>916.2733442123199</v>
       </c>
-    </row>
-    <row r="207" spans="1:12">
+      <c r="M206">
+        <v>60.88865441059153</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13">
       <c r="A207" s="1" t="s">
         <v>17</v>
       </c>
@@ -2812,8 +2815,11 @@
       <c r="L207">
         <v>616.1125544133573</v>
       </c>
-    </row>
-    <row r="208" spans="1:12">
+      <c r="M207">
+        <v>35.83983616600823</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13">
       <c r="A208" s="1" t="s">
         <v>18</v>
       </c>
@@ -2843,6 +2849,9 @@
       </c>
       <c r="L208">
         <v>632.8508658885638</v>
+      </c>
+      <c r="M208">
+        <v>62.74899949277329</v>
       </c>
     </row>
     <row r="209" spans="1:16">
@@ -2876,6 +2885,9 @@
       <c r="L209">
         <v>685.6402001475317</v>
       </c>
+      <c r="M209">
+        <v>39.27312093176155</v>
+      </c>
     </row>
     <row r="210" spans="1:16">
       <c r="A210" s="1" t="s">
@@ -2908,6 +2920,9 @@
       <c r="L210">
         <v>642.7512418990723</v>
       </c>
+      <c r="M210">
+        <v>32.45126239014346</v>
+      </c>
     </row>
     <row r="211" spans="1:16">
       <c r="A211" s="1" t="s">
@@ -2940,6 +2955,9 @@
       <c r="L211">
         <v>547.2762027671747</v>
       </c>
+      <c r="M211">
+        <v>48.68676002362864</v>
+      </c>
     </row>
     <row r="212" spans="1:16">
       <c r="A212" s="1" t="s">
@@ -2972,6 +2990,9 @@
       <c r="L212">
         <v>577.2938730650199</v>
       </c>
+      <c r="M212">
+        <v>29.8698997468404</v>
+      </c>
     </row>
     <row r="213" spans="1:16">
       <c r="A213" s="1" t="s">
@@ -3004,6 +3025,9 @@
       <c r="L213">
         <v>665.4653985962352</v>
       </c>
+      <c r="M213">
+        <v>18.15085844055914</v>
+      </c>
     </row>
     <row r="214" spans="1:16">
       <c r="A214" s="1" t="s">
@@ -3030,11 +3054,11 @@
       <c r="J214">
         <v>613.9074033720117</v>
       </c>
-      <c r="K214">
-        <v>176.1530890998578</v>
-      </c>
       <c r="L214">
         <v>1052.740935963408</v>
+      </c>
+      <c r="M214">
+        <v>176.1530890998578</v>
       </c>
     </row>
     <row r="215" spans="1:16">
@@ -3062,11 +3086,11 @@
       <c r="J215">
         <v>537.8133006804487</v>
       </c>
-      <c r="K215">
-        <v>187.9815228609831</v>
-      </c>
       <c r="L215">
         <v>975.4542706759576</v>
+      </c>
+      <c r="M215">
+        <v>187.9815228609831</v>
       </c>
     </row>
     <row r="216" spans="1:16">
@@ -3094,11 +3118,11 @@
       <c r="J216">
         <v>583.5352558129588</v>
       </c>
-      <c r="K216">
-        <v>233.7931264152482</v>
-      </c>
       <c r="L216">
         <v>1105.335216602344</v>
+      </c>
+      <c r="M216">
+        <v>233.7931264152482</v>
       </c>
     </row>
     <row r="217" spans="1:16">
@@ -3126,11 +3150,11 @@
       <c r="J217">
         <v>636.9120672958686</v>
       </c>
-      <c r="K217">
-        <v>182.822191121505</v>
-      </c>
       <c r="L217">
         <v>1069.582683515238</v>
+      </c>
+      <c r="M217">
+        <v>182.822191121505</v>
       </c>
     </row>
     <row r="218" spans="1:16">
@@ -3158,11 +3182,11 @@
       <c r="J218">
         <v>626.70549859147</v>
       </c>
-      <c r="K218">
-        <v>159.4572244667407</v>
-      </c>
       <c r="L218">
         <v>1068.637301838331</v>
+      </c>
+      <c r="M218">
+        <v>159.4572244667407</v>
       </c>
     </row>
     <row r="219" spans="1:16">
@@ -3190,11 +3214,11 @@
       <c r="J219">
         <v>409.5727621735166</v>
       </c>
-      <c r="K219">
-        <v>172.8555328955028</v>
-      </c>
       <c r="L219">
         <v>819.6675353116134</v>
+      </c>
+      <c r="M219">
+        <v>172.8555328955028</v>
       </c>
     </row>
     <row r="220" spans="1:16">
@@ -3222,11 +3246,11 @@
       <c r="J220">
         <v>551.7613064643763</v>
       </c>
-      <c r="K220">
-        <v>177.8358852147381</v>
-      </c>
       <c r="L220">
         <v>951.2881526218697</v>
+      </c>
+      <c r="M220">
+        <v>177.8358852147381</v>
       </c>
     </row>
     <row r="221" spans="1:16">
@@ -3254,11 +3278,11 @@
       <c r="J221">
         <v>653.1981231568413</v>
       </c>
-      <c r="K221">
-        <v>161.6355203723639</v>
-      </c>
       <c r="L221">
         <v>1074.995331305236</v>
+      </c>
+      <c r="M221">
+        <v>161.6355203723639</v>
       </c>
     </row>
     <row r="222" spans="1:16">
@@ -3281,16 +3305,16 @@
         <v>1166.524104503712</v>
       </c>
       <c r="M222">
+        <v>703.5126392194566</v>
+      </c>
+      <c r="N222">
         <v>556.6800000000001</v>
       </c>
-      <c r="N222">
+      <c r="O222">
         <v>0.03676612174277129</v>
       </c>
-      <c r="O222">
+      <c r="P222">
         <v>15163.62934093144</v>
-      </c>
-      <c r="P222">
-        <v>703.5126392194566</v>
       </c>
     </row>
     <row r="223" spans="1:16">
@@ -3313,16 +3337,16 @@
         <v>986.856369944623</v>
       </c>
       <c r="M223">
+        <v>608.7772152712714</v>
+      </c>
+      <c r="N223">
         <v>454.08</v>
       </c>
-      <c r="N223">
+      <c r="O223">
         <v>0.03880497512437811</v>
       </c>
-      <c r="O223">
+      <c r="P223">
         <v>11717.49185433488</v>
-      </c>
-      <c r="P223">
-        <v>608.7772152712714</v>
       </c>
     </row>
     <row r="224" spans="1:16">
@@ -3345,16 +3369,16 @@
         <v>1300.42401414824</v>
       </c>
       <c r="M224">
+        <v>921.1808561899852</v>
+      </c>
+      <c r="N224">
         <v>722.73</v>
       </c>
-      <c r="N224">
+      <c r="O224">
         <v>0.04016490147783251</v>
       </c>
-      <c r="O224">
+      <c r="P224">
         <v>17964.89661812995</v>
-      </c>
-      <c r="P224">
-        <v>921.1808561899852</v>
       </c>
     </row>
     <row r="225" spans="1:16">
@@ -3377,16 +3401,16 @@
         <v>1306.664805227499</v>
       </c>
       <c r="M225">
+        <v>839.9972294105689</v>
+      </c>
+      <c r="N225">
         <v>672.775</v>
       </c>
-      <c r="N225">
+      <c r="O225">
         <v>0.04215411928877849</v>
       </c>
-      <c r="O225">
+      <c r="P225">
         <v>15964.97578041526</v>
-      </c>
-      <c r="P225">
-        <v>839.9972294105689</v>
       </c>
     </row>
     <row r="226" spans="1:16">
@@ -3409,16 +3433,16 @@
         <v>1233.851840917993</v>
       </c>
       <c r="M226">
+        <v>750.1905916851415</v>
+      </c>
+      <c r="N226">
         <v>581.25</v>
       </c>
-      <c r="N226">
+      <c r="O226">
         <v>0.03782501593020121</v>
       </c>
-      <c r="O226">
+      <c r="P226">
         <v>15332.99248095844</v>
-      </c>
-      <c r="P226">
-        <v>750.1905916851415</v>
       </c>
     </row>
     <row r="227" spans="1:16">
@@ -3441,16 +3465,16 @@
         <v>1030.016075836826</v>
       </c>
       <c r="M227">
+        <v>734.534693277765</v>
+      </c>
+      <c r="N227">
         <v>581.71</v>
       </c>
-      <c r="N227">
+      <c r="O227">
         <v>0.0432</v>
       </c>
-      <c r="O227">
+      <c r="P227">
         <v>13478.15972223027</v>
-      </c>
-      <c r="P227">
-        <v>734.534693277765</v>
       </c>
     </row>
     <row r="228" spans="1:16">
@@ -3473,16 +3497,16 @@
         <v>1139.357067138913</v>
       </c>
       <c r="M228">
+        <v>755.278527670451</v>
+      </c>
+      <c r="N228">
         <v>608.0450000000001</v>
       </c>
-      <c r="N228">
+      <c r="O228">
         <v>0.03985358545090963</v>
       </c>
-      <c r="O228">
+      <c r="P228">
         <v>15257.67733593801</v>
-      </c>
-      <c r="P228">
-        <v>755.278527670451</v>
       </c>
     </row>
     <row r="229" spans="1:16">
@@ -3505,16 +3529,16 @@
         <v>959.1031170433897</v>
       </c>
       <c r="M229">
+        <v>561.5845682650163</v>
+      </c>
+      <c r="N229">
         <v>423.085</v>
       </c>
-      <c r="N229">
+      <c r="O229">
         <v>0.04355621890547264</v>
       </c>
-      <c r="O229">
+      <c r="P229">
         <v>9738.745902440323</v>
-      </c>
-      <c r="P229">
-        <v>561.5845682650163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>